<commit_message>
dynamic phasors expmples added
</commit_message>
<xml_diff>
--- a/grids/grid_uri/cigre/cigre_eu_lv_acdc/cigre_lv.xlsx
+++ b/grids/grid_uri/cigre/cigre_eu_lv_acdc/cigre_lv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmmau\workspace\pydae\examples\grids\grid_uri\cigre\cigre_eu_lv_acdc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmmau\workspace\pydae_examples\grids\grid_uri\cigre\cigre_eu_lv_acdc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A4BB18-5A7B-44D9-9213-F0E018B9C20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553A9CC5-8FC2-4367-BC31-0097AB6763D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10272" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cases" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="54">
   <si>
     <t>kVA</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Total C w/o 120kW:</t>
+  </si>
+  <si>
+    <t>¿o 2 AC?</t>
   </si>
 </sst>
 </file>
@@ -238,12 +241,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -258,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -270,12 +279,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,21 +601,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.15625" customWidth="1"/>
-    <col min="3" max="3" width="13.7890625" customWidth="1"/>
-    <col min="5" max="5" width="35.3125" customWidth="1"/>
-    <col min="6" max="6" width="35.578125" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
+    <col min="5" max="5" width="35.26953125" customWidth="1"/>
+    <col min="6" max="6" width="35.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
@@ -616,7 +627,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -630,7 +641,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -643,8 +654,11 @@
       <c r="E3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -658,7 +672,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -672,7 +686,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -687,24 +701,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.9453125" customWidth="1"/>
-    <col min="5" max="5" width="10.578125" customWidth="1"/>
-    <col min="11" max="11" width="11.9453125" customWidth="1"/>
+    <col min="1" max="2" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="2" t="s">
@@ -714,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -743,21 +757,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>200</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.95</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <f>C3*D3</f>
         <v>190</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <f>SQRT(C3*C3-E3*E3)</f>
         <v>62.44997998398398</v>
       </c>
@@ -766,7 +780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -776,11 +790,11 @@
       <c r="D4">
         <v>0.95</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="11">
         <f t="shared" ref="E4:E8" si="0">C4*D4</f>
         <v>14.25</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="11">
         <f t="shared" ref="F4:F8" si="1">SQRT(C4*C4-E4*E4)</f>
         <v>4.6837484987987983</v>
       </c>
@@ -788,14 +802,14 @@
       <c r="H4" t="s">
         <v>37</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="12">
         <v>0</v>
       </c>
       <c r="K4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -805,11 +819,11 @@
       <c r="D5">
         <v>0.95</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="11">
         <f t="shared" si="0"/>
         <v>49.4</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="11">
         <f t="shared" si="1"/>
         <v>16.236994795835844</v>
       </c>
@@ -817,14 +831,14 @@
       <c r="H5" t="s">
         <v>38</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="12">
         <v>0</v>
       </c>
       <c r="K5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -834,11 +848,11 @@
       <c r="D6">
         <v>0.95</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="11">
         <f t="shared" si="0"/>
         <v>52.25</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="11">
         <f t="shared" si="1"/>
         <v>17.173744495595596</v>
       </c>
@@ -846,14 +860,14 @@
       <c r="H6" t="s">
         <v>39</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="12">
         <v>0</v>
       </c>
       <c r="K6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -863,11 +877,11 @@
       <c r="D7">
         <v>0.95</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="11">
         <f t="shared" si="0"/>
         <v>33.25</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="11">
         <f t="shared" si="1"/>
         <v>10.928746497197197</v>
       </c>
@@ -875,14 +889,14 @@
       <c r="H7" t="s">
         <v>40</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="12">
         <v>0</v>
       </c>
       <c r="K7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -892,11 +906,11 @@
       <c r="D8">
         <v>0.95</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="11">
         <f t="shared" si="0"/>
         <v>44.65</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="11">
         <f t="shared" si="1"/>
         <v>14.675745296236238</v>
       </c>
@@ -904,14 +918,14 @@
       <c r="H8" t="s">
         <v>41</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="12">
         <v>0</v>
       </c>
       <c r="K8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -935,12 +949,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -964,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -974,11 +988,11 @@
       <c r="D12">
         <v>0.85</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="11">
         <f>C12*D12</f>
         <v>85</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="11">
         <f>SQRT(C12*C12-E12*E12)</f>
         <v>52.678268764263692</v>
       </c>
@@ -986,14 +1000,14 @@
       <c r="H12" t="s">
         <v>46</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="12">
         <v>0</v>
       </c>
       <c r="K12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1017,12 +1031,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -1046,30 +1060,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>120</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>0.9</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <f>C16*D16</f>
         <v>108</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <f>SQRT(C16*C16-E16*E16)</f>
         <v>52.306787322488084</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="8"/>
       <c r="K16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -1098,7 +1112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -1121,7 +1135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -1144,7 +1158,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1173,7 +1187,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -1196,7 +1210,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -1222,7 +1236,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -1251,7 +1265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -1268,14 +1282,14 @@
       </c>
       <c r="G24" s="3"/>
       <c r="I24" s="3">
-        <f t="shared" ref="E24:I24" si="4">SUM(I16:I23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="I24" si="4">SUM(I16:I23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1294,22 +1308,22 @@
       </c>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8">
         <f>SUM(E3:E8,E12,E16:E23)</f>
         <v>686.6</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="8">
         <f>SUM(F3:F8,F12,F16:F23)</f>
         <v>284.31258276559566</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1324,24 +1338,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA345F2-366F-45A0-B85B-520B2C20C240}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.9453125" customWidth="1"/>
-    <col min="5" max="5" width="10.578125" customWidth="1"/>
-    <col min="11" max="11" width="11.9453125" customWidth="1"/>
+    <col min="1" max="2" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="2" t="s">
@@ -1351,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1380,21 +1394,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>200</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.95</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <f>C3*D3</f>
         <v>190</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <f>SQRT(C3*C3-E3*E3)</f>
         <v>62.44997998398398</v>
       </c>
@@ -1403,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -1433,7 +1447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +1477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -1493,7 +1507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -1523,7 +1537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -1553,7 +1567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1577,12 +1591,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1606,7 +1620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -1636,7 +1650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1660,12 +1674,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -1689,30 +1703,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>120</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>0.9</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <f>C16*D16</f>
         <v>108</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <f>SQRT(C16*C16-E16*E16)</f>
         <v>52.306787322488084</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="8"/>
       <c r="K16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -1742,7 +1756,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -1766,7 +1780,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -1790,7 +1804,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -1820,7 +1834,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -1844,7 +1858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -1871,7 +1885,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -1901,7 +1915,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -1918,14 +1932,14 @@
       </c>
       <c r="G24" s="3"/>
       <c r="I24" s="3">
-        <f t="shared" ref="I24:M24" si="4">SUM(I16:I23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <f t="shared" ref="I24" si="4">SUM(I16:I23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1947,22 +1961,22 @@
         <v>1.4999999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8">
         <f>SUM(E3:E8,E12,E16:E23)</f>
         <v>880.9</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="8">
         <f>SUM(F3:F8,F12,F16:F23)</f>
         <v>369.0904904951575</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1975,26 +1989,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932038FD-EA30-401A-A7E3-21BC53F8B25D}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.9453125" customWidth="1"/>
-    <col min="5" max="5" width="10.578125" customWidth="1"/>
-    <col min="11" max="11" width="11.9453125" customWidth="1"/>
+    <col min="1" max="2" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="2" t="s">
@@ -2004,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2033,21 +2047,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>200</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.95</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <f>C3*D3</f>
         <v>190</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <f>SQRT(C3*C3-E3*E3)</f>
         <v>62.44997998398398</v>
       </c>
@@ -2056,7 +2070,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -2079,15 +2093,15 @@
       <c r="H4" t="s">
         <v>37</v>
       </c>
-      <c r="I4">
-        <f>'Case 0'!C4*Cases!$C$4</f>
-        <v>7.5</v>
+      <c r="I4" s="1">
+        <f>'Case 0'!E4*Cases!$C$4</f>
+        <v>7.125</v>
       </c>
       <c r="K4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -2110,15 +2124,15 @@
       <c r="H5" t="s">
         <v>38</v>
       </c>
-      <c r="I5">
-        <f>'Case 0'!C5*Cases!$C$4</f>
-        <v>26</v>
+      <c r="I5" s="1">
+        <f>'Case 0'!E5*Cases!$C$4</f>
+        <v>24.7</v>
       </c>
       <c r="K5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -2141,15 +2155,15 @@
       <c r="H6" t="s">
         <v>39</v>
       </c>
-      <c r="I6">
-        <f>'Case 0'!C6*Cases!$C$4</f>
-        <v>27.5</v>
+      <c r="I6" s="1">
+        <f>'Case 0'!E6*Cases!$C$4</f>
+        <v>26.125</v>
       </c>
       <c r="K6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -2172,15 +2186,15 @@
       <c r="H7" t="s">
         <v>40</v>
       </c>
-      <c r="I7">
-        <f>'Case 0'!C7*Cases!$C$4</f>
-        <v>17.5</v>
+      <c r="I7" s="1">
+        <f>'Case 0'!E7*Cases!$C$4</f>
+        <v>16.625</v>
       </c>
       <c r="K7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -2203,15 +2217,15 @@
       <c r="H8" t="s">
         <v>41</v>
       </c>
-      <c r="I8">
-        <f>'Case 0'!C8*Cases!$C$4</f>
-        <v>23.5</v>
+      <c r="I8" s="1">
+        <f>'Case 0'!E8*Cases!$C$4</f>
+        <v>22.324999999999999</v>
       </c>
       <c r="K8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2229,18 +2243,22 @@
       <c r="G9" s="3"/>
       <c r="I9" s="3">
         <f>SUM(I3:I8)</f>
-        <v>102</v>
+        <v>96.9</v>
       </c>
       <c r="K9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="M9" s="1">
+        <f>E9+I9</f>
+        <v>290.70000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2264,7 +2282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -2288,14 +2306,14 @@
         <v>46</v>
       </c>
       <c r="I12">
-        <f>'Case 0'!C12*Cases!$C$4</f>
-        <v>50</v>
+        <f>'Case 0'!E12*Cases!$C$4</f>
+        <v>42.5</v>
       </c>
       <c r="K12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2313,18 +2331,22 @@
       <c r="G13" s="3"/>
       <c r="I13" s="3">
         <f>SUM(I12:I12)</f>
-        <v>50</v>
+        <v>42.5</v>
       </c>
       <c r="K13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="M13" s="1">
+        <f>E13+I13</f>
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -2348,30 +2370,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>120</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>0.9</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <f>C16*D16</f>
         <v>108</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <f>SQRT(C16*C16-E16*E16)</f>
         <v>52.306787322488084</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="8"/>
       <c r="K16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -2395,14 +2417,14 @@
         <v>42</v>
       </c>
       <c r="I17">
-        <f>'Case 0'!C17*Cases!$C$4</f>
-        <v>10</v>
+        <f>2*'Case 0'!E17*Cases!$C$4</f>
+        <v>18</v>
       </c>
       <c r="K17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -2426,7 +2448,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -2450,7 +2472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -2474,14 +2496,14 @@
         <v>43</v>
       </c>
       <c r="I20">
-        <f>'Case 0'!C20*Cases!$C$4</f>
-        <v>12.5</v>
+        <f>2*'Case 0'!E20*Cases!$C$4</f>
+        <v>22.5</v>
       </c>
       <c r="K20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -2505,7 +2527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -2529,14 +2551,14 @@
         <v>44</v>
       </c>
       <c r="I22">
-        <f>'Case 0'!C22*Cases!$C$4</f>
-        <v>8</v>
+        <f>'Case 0'!E22*Cases!$C$4</f>
+        <v>7.2</v>
       </c>
       <c r="K22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -2560,14 +2582,14 @@
         <v>45</v>
       </c>
       <c r="I23">
-        <f>'Case 0'!C23*Cases!$C$4</f>
-        <v>4</v>
+        <f>2*'Case 0'!E23*Cases!$C$4</f>
+        <v>7.2</v>
       </c>
       <c r="K23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -2585,13 +2607,17 @@
       <c r="G24" s="3"/>
       <c r="I24" s="3">
         <f>SUM(I16:I23)</f>
-        <v>34.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>54.900000000000006</v>
+      </c>
+      <c r="M24" s="1">
+        <f>E24+I24</f>
+        <v>164.70000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -2606,29 +2632,29 @@
       <c r="G26" s="3"/>
       <c r="I26" s="3">
         <f>I9+I13+I24</f>
-        <v>186.5</v>
+        <v>194.3</v>
       </c>
       <c r="K26" s="3">
         <f>(E26+I26)/'Case 0'!E26</f>
-        <v>1.4799279464745239</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+        <v>1.5000000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9">
-        <f>SUM(E3:E8,E12,E16:E23)</f>
-        <v>686.6</v>
-      </c>
-      <c r="F27" s="9">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8">
+        <f>SUM(E3:E8,E12,E16:E23)+I26</f>
+        <v>880.90000000000009</v>
+      </c>
+      <c r="F27" s="8">
         <f>SUM(F3:F8,F12,F16:F23)</f>
         <v>284.31258276559566</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2643,24 +2669,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCA3ECB-F2EA-440D-9208-227E0550706D}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="13.9453125" customWidth="1"/>
-    <col min="5" max="5" width="10.578125" customWidth="1"/>
-    <col min="11" max="11" width="11.9453125" customWidth="1"/>
+    <col min="1" max="2" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="2" t="s">
@@ -2670,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -2699,21 +2725,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>200</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.95</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <f>C3*D3</f>
         <v>190</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <f>SQRT(C3*C3-E3*E3)</f>
         <v>62.44997998398398</v>
       </c>
@@ -2722,7 +2748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -2753,7 +2779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>21</v>
       </c>
@@ -2784,7 +2810,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -2815,7 +2841,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>23</v>
       </c>
@@ -2846,7 +2872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -2877,7 +2903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -2901,12 +2927,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2930,7 +2956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -2961,7 +2987,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -2985,12 +3011,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -3014,30 +3040,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>120</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>0.9</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <f>C16*D16</f>
         <v>108</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="8">
         <f>SQRT(C16*C16-E16*E16)</f>
         <v>52.306787322488084</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="8"/>
       <c r="K16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>12</v>
       </c>
@@ -3068,7 +3094,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>13</v>
       </c>
@@ -3092,7 +3118,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>14</v>
       </c>
@@ -3116,7 +3142,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>15</v>
       </c>
@@ -3147,7 +3173,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>16</v>
       </c>
@@ -3171,7 +3197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -3202,7 +3228,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>18</v>
       </c>
@@ -3233,7 +3259,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -3254,10 +3280,10 @@
         <v>82.8</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -3279,22 +3305,22 @@
         <v>1.4518270715388575</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9">
-        <f>SUM(E3:E8,E12,E16:E23)</f>
-        <v>414.58</v>
-      </c>
-      <c r="F27" s="9">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8">
+        <f>SUM(E3:E8,E12,E16:E23)+SUM(I4:I8,I12,I17:I23)</f>
+        <v>862.18000000000006</v>
+      </c>
+      <c r="F27" s="8">
         <f>SUM(F3:F8,F12,F16:F23)</f>
         <v>165.62351194420913</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>